<commit_message>
Update reports - 2026-01-27 10:10
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="199">
   <si>
     <t>Publication ID</t>
   </si>
@@ -553,6 +553,9 @@
   </si>
   <si>
     <t>51226, 51210, 51224, 51227, 51183, 51167, 51128, 51102, 51113, 51123, 51065, 51117, 51109, 51069, 51066, 51012, 50888, 51003, 51008, 50887, 50890, 50845, 50844, 50872, 50873, 50850, 50843, 50806, 50761, 50723, 50681, 50724, 50721, 50700, 50718, 50719, 50720, 50709, 50711, 50713, 50722, 50674, 50676, 50677, 50678, 50679, 50685, 50625, 50626, 50624</t>
+  </si>
+  <si>
+    <t>10:10:11</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -677,8 +680,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C2" totalsRowShown="0">
-  <autoFilter ref="A1:C2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C3" totalsRowShown="0">
+  <autoFilter ref="A1:C3"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -689,8 +692,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Order_Papers" displayName="Order_Papers" ref="A1:H5" totalsRowShown="0">
-  <autoFilter ref="A1:H5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Order_Papers" displayName="Order_Papers" ref="A1:H9" totalsRowShown="0">
+  <autoFilter ref="A1:H9"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Order Paper date"/>
     <tableColumn id="2" name="Committee name"/>
@@ -2025,7 +2028,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2051,6 +2054,14 @@
       </c>
       <c r="C2" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2063,7 +2074,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2071,28 +2082,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2100,10 +2111,10 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
@@ -2120,13 +2131,13 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E3" t="s">
         <v>38</v>
@@ -2140,13 +2151,13 @@
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E4" t="s">
         <v>38</v>
@@ -2160,19 +2171,99 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E5" t="s">
         <v>38</v>
       </c>
       <c r="F5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" t="s">
         <v>197</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-27 10:21
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="202">
   <si>
     <t>Publication ID</t>
   </si>
@@ -558,6 +558,9 @@
     <t>10:10:11</t>
   </si>
   <si>
+    <t>10:21:34</t>
+  </si>
+  <si>
     <t>Order Paper date</t>
   </si>
   <si>
@@ -585,6 +588,9 @@
     <t>5th Report: First 1000 Days: a renewed focus</t>
   </si>
   <si>
+    <t>Published</t>
+  </si>
+  <si>
     <t>International Development</t>
   </si>
   <si>
@@ -592,6 +598,9 @@
   </si>
   <si>
     <t>HC 1626</t>
+  </si>
+  <si>
+    <t>Missing</t>
   </si>
   <si>
     <t>Treasury</t>
@@ -680,8 +689,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -692,8 +701,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Order_Papers" displayName="Order_Papers" ref="A1:H9" totalsRowShown="0">
-  <autoFilter ref="A1:H9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Order_Papers" displayName="Order_Papers" ref="A1:H13" totalsRowShown="0">
+  <autoFilter ref="A1:H13"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Order Paper date"/>
     <tableColumn id="2" name="Committee name"/>
@@ -2028,7 +2037,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2062,6 +2071,14 @@
       </c>
       <c r="B3" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2074,7 +2091,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2082,28 +2099,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2111,10 +2128,10 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
@@ -2124,6 +2141,9 @@
       </c>
       <c r="F2" t="s">
         <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2131,19 +2151,22 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
         <v>38</v>
       </c>
       <c r="F3" t="s">
         <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2151,19 +2174,22 @@
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C4" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D4" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E4" t="s">
         <v>38</v>
       </c>
       <c r="F4" t="s">
         <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2171,19 +2197,22 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E5" t="s">
         <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>198</v>
+        <v>201</v>
+      </c>
+      <c r="G5" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2191,10 +2220,10 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
@@ -2204,6 +2233,9 @@
       </c>
       <c r="F6" t="s">
         <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2211,19 +2243,22 @@
         <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C7" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D7" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E7" t="s">
         <v>38</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2231,19 +2266,22 @@
         <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C8" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D8" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E8" t="s">
         <v>38</v>
       </c>
       <c r="F8" t="s">
         <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2251,19 +2289,114 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C9" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D9" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E9" t="s">
         <v>38</v>
       </c>
       <c r="F9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>191</v>
+      </c>
+      <c r="C11" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" t="s">
+        <v>197</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
         <v>198</v>
+      </c>
+      <c r="C13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>201</v>
+      </c>
+      <c r="G13" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-27 11:47
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="163">
   <si>
     <t>Publication ID</t>
   </si>
@@ -454,6 +454,9 @@
   </si>
   <si>
     <t>51245, 51246, 51226, 51228, 51210, 51224, 51227, 51202, 51183, 51188, 51189, 51209, 51129, 51167, 51128, 51102, 51113, 51123, 51065, 51076, 51117, 51109, 51068, 51063, 51069, 51066, 51014, 51012, 50888, 50979</t>
+  </si>
+  <si>
+    <t>11:47:03</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -569,8 +572,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C2" totalsRowShown="0">
-  <autoFilter ref="A1:C2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C3" totalsRowShown="0">
+  <autoFilter ref="A1:C3"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -1689,7 +1692,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1715,6 +1718,14 @@
       </c>
       <c r="C2" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1735,28 +1746,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1764,10 +1775,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -1779,7 +1790,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1787,10 +1798,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -1802,7 +1813,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1810,10 +1821,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -1825,7 +1836,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1833,10 +1844,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -1848,7 +1859,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-27 14:06
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="166">
   <si>
     <t>Publication ID</t>
   </si>
@@ -459,6 +459,9 @@
     <t>11:47:03</t>
   </si>
   <si>
+    <t>14:06:30</t>
+  </si>
+  <si>
     <t>Order Paper date</t>
   </si>
   <si>
@@ -505,6 +508,12 @@
   </si>
   <si>
     <t>3rd Special Report: The Home Office’s management of asylum accommodation: Government Response</t>
+  </si>
+  <si>
+    <t>Women and Equalities</t>
+  </si>
+  <si>
+    <t>8th Special Report: Female entrepreneurship: Government Response</t>
   </si>
 </sst>
 </file>
@@ -572,8 +581,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -584,8 +593,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Order_Papers" displayName="Order_Papers" ref="A1:H5" totalsRowShown="0">
-  <autoFilter ref="A1:H5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Order_Papers" displayName="Order_Papers" ref="A1:H6" totalsRowShown="0">
+  <autoFilter ref="A1:H6"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Order Paper date"/>
     <tableColumn id="2" name="Committee name"/>
@@ -1692,7 +1701,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1726,6 +1735,14 @@
       </c>
       <c r="B3" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1738,7 +1755,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1746,28 +1763,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1775,10 +1792,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -1790,7 +1807,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1798,10 +1815,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -1813,7 +1830,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1821,10 +1838,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -1836,7 +1853,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1844,10 +1861,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -1859,7 +1876,30 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>156</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-27 14:11
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="167">
   <si>
     <t>Publication ID</t>
   </si>
@@ -460,6 +460,9 @@
   </si>
   <si>
     <t>14:06:30</t>
+  </si>
+  <si>
+    <t>14:11:28</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -581,8 +584,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C5" totalsRowShown="0">
+  <autoFilter ref="A1:C5"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -1701,7 +1704,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1743,6 +1746,14 @@
       </c>
       <c r="B4" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1763,28 +1774,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1792,10 +1803,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -1807,7 +1818,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1815,10 +1826,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -1830,7 +1841,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1838,10 +1849,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -1853,7 +1864,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1861,10 +1872,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -1876,7 +1887,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1884,10 +1895,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -1899,7 +1910,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-28 00:21
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="176">
   <si>
     <t>Publication ID</t>
   </si>
@@ -465,6 +465,12 @@
     <t>14:11:28</t>
   </si>
   <si>
+    <t>2026-01-28</t>
+  </si>
+  <si>
+    <t>00:21:31</t>
+  </si>
+  <si>
     <t>Order Paper date</t>
   </si>
   <si>
@@ -517,6 +523,27 @@
   </si>
   <si>
     <t>8th Special Report: Female entrepreneurship: Government Response</t>
+  </si>
+  <si>
+    <t>Public Accounts</t>
+  </si>
+  <si>
+    <t>63rd Report: Increasing police productivity</t>
+  </si>
+  <si>
+    <t>HC 1239</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>5th Report: Engine for growth: securing skills for transport manufacturing</t>
+  </si>
+  <si>
+    <t>HC 1223</t>
   </si>
 </sst>
 </file>
@@ -584,8 +611,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -596,8 +623,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Order_Papers" displayName="Order_Papers" ref="A1:H6" totalsRowShown="0">
-  <autoFilter ref="A1:H6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Order_Papers" displayName="Order_Papers" ref="A1:H8" totalsRowShown="0">
+  <autoFilter ref="A1:H8"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Order Paper date"/>
     <tableColumn id="2" name="Committee name"/>
@@ -1704,7 +1731,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1754,6 +1781,14 @@
       </c>
       <c r="B5" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1766,7 +1801,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1774,28 +1809,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1803,10 +1838,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -1818,7 +1853,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1826,10 +1861,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -1841,7 +1876,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1849,10 +1884,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -1864,7 +1899,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1872,10 +1907,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -1887,7 +1922,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1895,10 +1930,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -1910,7 +1945,53 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>158</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-28 00:25
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="177">
   <si>
     <t>Publication ID</t>
   </si>
@@ -469,6 +469,9 @@
   </si>
   <si>
     <t>00:21:31</t>
+  </si>
+  <si>
+    <t>00:25:10</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -611,8 +614,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C6" totalsRowShown="0">
-  <autoFilter ref="A1:C6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C7" totalsRowShown="0">
+  <autoFilter ref="A1:C7"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -1731,7 +1734,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1789,6 +1792,14 @@
       </c>
       <c r="B6" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1809,28 +1820,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1838,10 +1849,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -1853,7 +1864,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1861,10 +1872,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -1876,7 +1887,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1884,10 +1895,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -1899,7 +1910,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1907,10 +1918,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -1922,7 +1933,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1930,10 +1941,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -1945,7 +1956,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1953,13 +1964,13 @@
         <v>149</v>
       </c>
       <c r="B7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E7" t="s">
         <v>149</v>
@@ -1968,7 +1979,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1976,13 +1987,13 @@
         <v>149</v>
       </c>
       <c r="B8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E8" t="s">
         <v>149</v>
@@ -1991,7 +2002,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-28 04:11
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="188">
   <si>
     <t>Publication ID</t>
   </si>
@@ -441,6 +441,39 @@
     <t>Tackling the drugs crisis in our prisons: Government Response</t>
   </si>
   <si>
+    <t>51276</t>
+  </si>
+  <si>
+    <t>HC 1239</t>
+  </si>
+  <si>
+    <t>Increasing police productivity</t>
+  </si>
+  <si>
+    <t>63rd Report</t>
+  </si>
+  <si>
+    <t>2026-01-28</t>
+  </si>
+  <si>
+    <t>0:20:31</t>
+  </si>
+  <si>
+    <t>4:10:36</t>
+  </si>
+  <si>
+    <t>51283</t>
+  </si>
+  <si>
+    <t>HC 1234</t>
+  </si>
+  <si>
+    <t>Transport Committee</t>
+  </si>
+  <si>
+    <t>Engine for growth: securing skills for transport manufacturing</t>
+  </si>
+  <si>
     <t>Scan date</t>
   </si>
   <si>
@@ -465,15 +498,18 @@
     <t>14:11:28</t>
   </si>
   <si>
-    <t>2026-01-28</t>
-  </si>
-  <si>
     <t>00:21:31</t>
   </si>
   <si>
     <t>00:25:10</t>
   </si>
   <si>
+    <t>04:11:36</t>
+  </si>
+  <si>
+    <t>51276, 51283, 51285</t>
+  </si>
+  <si>
     <t>Order Paper date</t>
   </si>
   <si>
@@ -534,19 +570,16 @@
     <t>63rd Report: Increasing police productivity</t>
   </si>
   <si>
-    <t>HC 1239</t>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>5th Report: Engine for growth: securing skills for transport manufacturing</t>
+  </si>
+  <si>
+    <t>HC 1223</t>
   </si>
   <si>
     <t>Missing</t>
-  </si>
-  <si>
-    <t>Transport</t>
-  </si>
-  <si>
-    <t>5th Report: Engine for growth: securing skills for transport manufacturing</t>
-  </si>
-  <si>
-    <t>HC 1223</t>
   </si>
 </sst>
 </file>
@@ -594,8 +627,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reports" displayName="Reports" ref="A1:K25" totalsRowShown="0">
-  <autoFilter ref="A1:K25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reports" displayName="Reports" ref="A1:K27" totalsRowShown="0">
+  <autoFilter ref="A1:K27"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Publication ID"/>
     <tableColumn id="2" name="HC Number"/>
@@ -614,8 +647,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C7" totalsRowShown="0">
-  <autoFilter ref="A1:C7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C8" totalsRowShown="0">
+  <autoFilter ref="A1:C8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -927,7 +960,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1722,6 +1755,76 @@
       </c>
       <c r="K25" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
+        <v>143</v>
+      </c>
+      <c r="G26" t="s">
+        <v>144</v>
+      </c>
+      <c r="H26" t="s">
+        <v>145</v>
+      </c>
+      <c r="I26" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" t="s">
+        <v>146</v>
+      </c>
+      <c r="K26" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
+        <v>148</v>
+      </c>
+      <c r="B27" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s">
+        <v>151</v>
+      </c>
+      <c r="G27" t="s">
+        <v>59</v>
+      </c>
+      <c r="H27" t="s">
+        <v>145</v>
+      </c>
+      <c r="I27" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" t="s">
+        <v>146</v>
+      </c>
+      <c r="K27" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1734,7 +1837,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1742,13 +1845,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1756,10 +1859,10 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1767,7 +1870,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1775,7 +1878,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1783,23 +1886,34 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1820,28 +1934,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="B1" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="C1" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="F1" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="G1" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="H1" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1849,10 +1963,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -1864,7 +1978,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1872,10 +1986,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -1887,7 +2001,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1895,10 +2009,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -1910,7 +2024,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1918,10 +2032,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -1933,7 +2047,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1941,10 +2055,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -1956,24 +2070,24 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="D7" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="E7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -1984,25 +2098,25 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="D8" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="E8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-28 09:59
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="189">
   <si>
     <t>Publication ID</t>
   </si>
@@ -508,6 +508,9 @@
   </si>
   <si>
     <t>51276, 51283, 51285</t>
+  </si>
+  <si>
+    <t>09:59:49</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -647,8 +650,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C8" totalsRowShown="0">
-  <autoFilter ref="A1:C8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C9" totalsRowShown="0">
+  <autoFilter ref="A1:C9"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -1837,7 +1840,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1914,6 +1917,14 @@
       </c>
       <c r="C8" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1934,28 +1945,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1963,10 +1974,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -1978,7 +1989,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1986,10 +1997,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -2001,7 +2012,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2009,10 +2020,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -2024,7 +2035,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2032,10 +2043,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -2047,7 +2058,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2055,10 +2066,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2070,7 +2081,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2078,10 +2089,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D7" t="s">
         <v>142</v>
@@ -2093,7 +2104,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2101,13 +2112,13 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E8" t="s">
         <v>145</v>
@@ -2116,7 +2127,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-28 11:45
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="191">
   <si>
     <t>Publication ID</t>
   </si>
@@ -511,6 +511,12 @@
   </si>
   <si>
     <t>09:59:49</t>
+  </si>
+  <si>
+    <t>11:45:28</t>
+  </si>
+  <si>
+    <t>51302</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -650,8 +656,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -1840,7 +1846,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1925,6 +1931,17 @@
       </c>
       <c r="B9" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1945,28 +1962,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1974,10 +1991,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -1989,7 +2006,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1997,10 +2014,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -2012,7 +2029,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2020,10 +2037,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C4" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -2035,7 +2052,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2043,10 +2060,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -2058,7 +2075,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2066,10 +2083,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2081,7 +2098,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2089,10 +2106,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D7" t="s">
         <v>142</v>
@@ -2104,7 +2121,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2112,13 +2129,13 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C8" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E8" t="s">
         <v>145</v>
@@ -2127,7 +2144,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-29 00:47
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="193">
   <si>
     <t>Publication ID</t>
   </si>
@@ -517,6 +517,12 @@
   </si>
   <si>
     <t>51302</t>
+  </si>
+  <si>
+    <t>2026-01-29</t>
+  </si>
+  <si>
+    <t>00:47:17</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -656,8 +662,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C10" totalsRowShown="0">
-  <autoFilter ref="A1:C10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C11" totalsRowShown="0">
+  <autoFilter ref="A1:C11"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -1846,7 +1852,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1942,6 +1948,14 @@
       </c>
       <c r="C10" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1962,28 +1976,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1991,10 +2005,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2006,7 +2020,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2014,10 +2028,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -2029,7 +2043,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2037,10 +2051,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -2052,7 +2066,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2060,10 +2074,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -2075,7 +2089,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2083,10 +2097,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2098,7 +2112,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2106,10 +2120,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D7" t="s">
         <v>142</v>
@@ -2121,7 +2135,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2129,13 +2143,13 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D8" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E8" t="s">
         <v>145</v>
@@ -2144,7 +2158,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-29 04:55
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="194">
   <si>
     <t>Publication ID</t>
   </si>
@@ -523,6 +523,9 @@
   </si>
   <si>
     <t>00:47:17</t>
+  </si>
+  <si>
+    <t>04:55:27</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -662,8 +665,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C11" totalsRowShown="0">
-  <autoFilter ref="A1:C11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C12" totalsRowShown="0">
+  <autoFilter ref="A1:C12"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -1852,7 +1855,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1956,6 +1959,14 @@
       </c>
       <c r="B11" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1976,28 +1987,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2005,10 +2016,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2020,7 +2031,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2028,10 +2039,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -2043,7 +2054,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2051,10 +2062,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -2066,7 +2077,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2074,10 +2085,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -2089,7 +2100,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2097,10 +2108,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2112,7 +2123,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2120,10 +2131,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D7" t="s">
         <v>142</v>
@@ -2135,7 +2146,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2143,13 +2154,13 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E8" t="s">
         <v>145</v>
@@ -2158,7 +2169,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-29 11:05
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="196">
   <si>
     <t>Publication ID</t>
   </si>
@@ -526,6 +526,12 @@
   </si>
   <si>
     <t>04:55:27</t>
+  </si>
+  <si>
+    <t>11:05:03</t>
+  </si>
+  <si>
+    <t>51335</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -665,8 +671,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C12" totalsRowShown="0">
-  <autoFilter ref="A1:C12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C13" totalsRowShown="0">
+  <autoFilter ref="A1:C13"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -1855,7 +1861,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1967,6 +1973,17 @@
       </c>
       <c r="B12" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1987,28 +2004,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="G1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2016,10 +2033,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2031,7 +2048,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2039,10 +2056,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -2054,7 +2071,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2062,10 +2079,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -2077,7 +2094,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2085,10 +2102,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -2100,7 +2117,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2108,10 +2125,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2123,7 +2140,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2131,10 +2148,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C7" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
         <v>142</v>
@@ -2146,7 +2163,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2154,13 +2171,13 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C8" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E8" t="s">
         <v>145</v>
@@ -2169,7 +2186,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-29 11:57
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="197">
   <si>
     <t>Publication ID</t>
   </si>
@@ -532,6 +532,9 @@
   </si>
   <si>
     <t>51335</t>
+  </si>
+  <si>
+    <t>11:57:55</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -671,8 +674,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C13" totalsRowShown="0">
-  <autoFilter ref="A1:C13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C14" totalsRowShown="0">
+  <autoFilter ref="A1:C14"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -1861,7 +1864,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1984,6 +1987,14 @@
       </c>
       <c r="C13" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2004,28 +2015,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2033,10 +2044,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2048,7 +2059,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2056,10 +2067,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -2071,7 +2082,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2079,10 +2090,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -2094,7 +2105,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2102,10 +2113,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -2117,7 +2128,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2125,10 +2136,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2140,7 +2151,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2148,10 +2159,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D7" t="s">
         <v>142</v>
@@ -2163,7 +2174,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2171,13 +2182,13 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E8" t="s">
         <v>145</v>
@@ -2186,7 +2197,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-30 00:03
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="216">
   <si>
     <t>Publication ID</t>
   </si>
@@ -474,6 +474,57 @@
     <t>Engine for growth: securing skills for transport manufacturing</t>
   </si>
   <si>
+    <t>51305</t>
+  </si>
+  <si>
+    <t>HC 571</t>
+  </si>
+  <si>
+    <t>Discrimination, harassment and abuse against Muslim women</t>
+  </si>
+  <si>
+    <t>10th Report</t>
+  </si>
+  <si>
+    <t>2026-01-30</t>
+  </si>
+  <si>
+    <t>0:02:50</t>
+  </si>
+  <si>
+    <t>51310</t>
+  </si>
+  <si>
+    <t>Large Print – 10th Report – Discrimination, harassment and abuse against Muslim women</t>
+  </si>
+  <si>
+    <t>51330</t>
+  </si>
+  <si>
+    <t>HC 1639</t>
+  </si>
+  <si>
+    <t>Ending the cycle of reoffending – part one: rehabilitation in prisons: Government Response</t>
+  </si>
+  <si>
+    <t>51334</t>
+  </si>
+  <si>
+    <t>Costs of clinical negligence</t>
+  </si>
+  <si>
+    <t>64th Report</t>
+  </si>
+  <si>
+    <t>51344</t>
+  </si>
+  <si>
+    <t>HC 1651</t>
+  </si>
+  <si>
+    <t>The work of the Committee in 2024-25, and Industrial transition in Scotland</t>
+  </si>
+  <si>
     <t>Scan date</t>
   </si>
   <si>
@@ -535,6 +586,12 @@
   </si>
   <si>
     <t>11:57:55</t>
+  </si>
+  <si>
+    <t>00:03:50</t>
+  </si>
+  <si>
+    <t>51305, 51310, 51330, 51334, 51344</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -654,8 +711,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reports" displayName="Reports" ref="A1:K27" totalsRowShown="0">
-  <autoFilter ref="A1:K27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reports" displayName="Reports" ref="A1:K32" totalsRowShown="0">
+  <autoFilter ref="A1:K32"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Publication ID"/>
     <tableColumn id="2" name="HC Number"/>
@@ -674,8 +731,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C14" totalsRowShown="0">
-  <autoFilter ref="A1:C14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C15" totalsRowShown="0">
+  <autoFilter ref="A1:C15"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -987,7 +1044,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1852,6 +1909,163 @@
       </c>
       <c r="K27" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>154</v>
+      </c>
+      <c r="G28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H28" t="s">
+        <v>156</v>
+      </c>
+      <c r="I28" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" t="s">
+        <v>159</v>
+      </c>
+      <c r="H29" t="s">
+        <v>156</v>
+      </c>
+      <c r="I29" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" t="s">
+        <v>161</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" t="s">
+        <v>162</v>
+      </c>
+      <c r="G30" t="s">
+        <v>77</v>
+      </c>
+      <c r="H30" t="s">
+        <v>156</v>
+      </c>
+      <c r="I30" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>164</v>
+      </c>
+      <c r="G31" t="s">
+        <v>165</v>
+      </c>
+      <c r="H31" t="s">
+        <v>156</v>
+      </c>
+      <c r="I31" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" t="s">
+        <v>168</v>
+      </c>
+      <c r="G32" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" t="s">
+        <v>156</v>
+      </c>
+      <c r="I32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K32" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1864,7 +2078,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1872,13 +2086,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1886,10 +2100,10 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1897,7 +2111,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1905,7 +2119,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1913,7 +2127,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1921,7 +2135,7 @@
         <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1929,7 +2143,7 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1937,10 +2151,10 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="C8" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1948,7 +2162,7 @@
         <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1956,45 +2170,56 @@
         <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="C10" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="B11" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="B13" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="C13" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="B14" t="s">
-        <v>172</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B15" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2015,28 +2240,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="C1" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="F1" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="G1" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="H1" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2044,10 +2269,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2059,7 +2284,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2067,10 +2292,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="C3" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -2082,7 +2307,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2090,10 +2315,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -2105,7 +2330,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2113,10 +2338,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="C5" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -2128,7 +2353,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2136,10 +2361,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2151,7 +2376,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2159,10 +2384,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="C7" t="s">
-        <v>192</v>
+        <v>211</v>
       </c>
       <c r="D7" t="s">
         <v>142</v>
@@ -2174,7 +2399,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2182,13 +2407,13 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="C8" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="D8" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="E8" t="s">
         <v>145</v>
@@ -2197,7 +2422,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-30 04:59
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="217">
   <si>
     <t>Publication ID</t>
   </si>
@@ -592,6 +592,9 @@
   </si>
   <si>
     <t>51305, 51310, 51330, 51334, 51344</t>
+  </si>
+  <si>
+    <t>04:59:36</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -731,8 +734,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C15" totalsRowShown="0">
-  <autoFilter ref="A1:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C16" totalsRowShown="0">
+  <autoFilter ref="A1:C16"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -2078,7 +2081,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2220,6 +2223,14 @@
       </c>
       <c r="C15" t="s">
         <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2240,28 +2251,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2269,10 +2280,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2284,7 +2295,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2292,10 +2303,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -2307,7 +2318,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2315,10 +2326,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -2330,7 +2341,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2338,10 +2349,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -2353,7 +2364,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2361,10 +2372,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2376,7 +2387,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2384,10 +2395,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D7" t="s">
         <v>142</v>
@@ -2399,7 +2410,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2407,13 +2418,13 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E8" t="s">
         <v>145</v>
@@ -2422,7 +2433,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-30 09:55
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="224">
   <si>
     <t>Publication ID</t>
   </si>
@@ -525,6 +525,24 @@
     <t>The work of the Committee in 2024-25, and Industrial transition in Scotland</t>
   </si>
   <si>
+    <t>51312</t>
+  </si>
+  <si>
+    <t>HC 785</t>
+  </si>
+  <si>
+    <t>Welsh Affairs Committee</t>
+  </si>
+  <si>
+    <t>Farming in Wales in 2025: Challenges and Opportunities: Government Response</t>
+  </si>
+  <si>
+    <t>09:00:00</t>
+  </si>
+  <si>
+    <t>0:55:18</t>
+  </si>
+  <si>
     <t>Scan date</t>
   </si>
   <si>
@@ -595,6 +613,9 @@
   </si>
   <si>
     <t>04:59:36</t>
+  </si>
+  <si>
+    <t>09:55:18</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -714,8 +735,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reports" displayName="Reports" ref="A1:K32" totalsRowShown="0">
-  <autoFilter ref="A1:K32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reports" displayName="Reports" ref="A1:K33" totalsRowShown="0">
+  <autoFilter ref="A1:K33"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Publication ID"/>
     <tableColumn id="2" name="HC Number"/>
@@ -734,8 +755,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C16" totalsRowShown="0">
-  <autoFilter ref="A1:C16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C17" totalsRowShown="0">
+  <autoFilter ref="A1:C17"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -1047,7 +1068,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2069,6 +2090,38 @@
       </c>
       <c r="K32" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>171</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" t="s">
+        <v>172</v>
+      </c>
+      <c r="G33" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" t="s">
+        <v>156</v>
+      </c>
+      <c r="I33" t="s">
+        <v>173</v>
+      </c>
+      <c r="K33" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2081,7 +2134,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2089,13 +2142,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2103,10 +2156,10 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2114,7 +2167,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2122,7 +2175,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2130,7 +2183,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2138,7 +2191,7 @@
         <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2146,7 +2199,7 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2154,10 +2207,10 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2165,7 +2218,7 @@
         <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2173,45 +2226,45 @@
         <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B11" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B12" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B13" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C13" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B14" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2219,10 +2272,10 @@
         <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C15" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2230,7 +2283,18 @@
         <v>156</v>
       </c>
       <c r="B16" t="s">
-        <v>192</v>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C17" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2251,28 +2315,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C1" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="F1" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="G1" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="H1" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2280,10 +2344,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2295,7 +2359,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2303,10 +2367,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -2318,7 +2382,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2326,10 +2390,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="C4" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -2341,7 +2405,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2349,10 +2413,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="C5" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -2364,7 +2428,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2372,10 +2436,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="C6" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2387,7 +2451,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2395,10 +2459,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D7" t="s">
         <v>142</v>
@@ -2410,7 +2474,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2418,13 +2482,13 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="D8" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="E8" t="s">
         <v>145</v>
@@ -2433,7 +2497,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-30 09:57
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="225">
   <si>
     <t>Publication ID</t>
   </si>
@@ -616,6 +616,9 @@
   </si>
   <si>
     <t>09:55:18</t>
+  </si>
+  <si>
+    <t>09:57:42</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -755,8 +758,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C17" totalsRowShown="0">
-  <autoFilter ref="A1:C17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C18" totalsRowShown="0">
+  <autoFilter ref="A1:C18"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -2134,7 +2137,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2295,6 +2298,14 @@
       </c>
       <c r="C17" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2315,28 +2326,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2344,10 +2355,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2359,7 +2370,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2367,10 +2378,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -2382,7 +2393,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2390,10 +2401,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -2405,7 +2416,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2413,10 +2424,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -2428,7 +2439,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2436,10 +2447,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2451,7 +2462,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2459,10 +2470,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D7" t="s">
         <v>142</v>
@@ -2474,7 +2485,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2482,13 +2493,13 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E8" t="s">
         <v>145</v>
@@ -2497,7 +2508,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-30 10:12
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="226">
   <si>
     <t>Publication ID</t>
   </si>
@@ -619,6 +619,9 @@
   </si>
   <si>
     <t>09:57:42</t>
+  </si>
+  <si>
+    <t>10:12:42</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -758,8 +761,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C18" totalsRowShown="0">
-  <autoFilter ref="A1:C18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C19" totalsRowShown="0">
+  <autoFilter ref="A1:C19"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -2137,7 +2140,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2306,6 +2309,14 @@
       </c>
       <c r="B18" t="s">
         <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2326,28 +2337,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2355,10 +2366,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2370,7 +2381,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2378,10 +2389,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -2393,7 +2404,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2401,10 +2412,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -2416,7 +2427,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2424,10 +2435,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -2439,7 +2450,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2447,10 +2458,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2462,7 +2473,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2470,10 +2481,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D7" t="s">
         <v>142</v>
@@ -2485,7 +2496,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2493,13 +2504,13 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E8" t="s">
         <v>145</v>
@@ -2508,7 +2519,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-30 10:59
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="227">
   <si>
     <t>Publication ID</t>
   </si>
@@ -622,6 +622,9 @@
   </si>
   <si>
     <t>10:12:42</t>
+  </si>
+  <si>
+    <t>10:59:37</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -761,8 +764,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C19" totalsRowShown="0">
-  <autoFilter ref="A1:C19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C20" totalsRowShown="0">
+  <autoFilter ref="A1:C20"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -2140,7 +2143,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2317,6 +2320,14 @@
       </c>
       <c r="B19" t="s">
         <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2337,28 +2348,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2366,10 +2377,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2381,7 +2392,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2389,10 +2400,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -2404,7 +2415,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2412,10 +2423,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -2427,7 +2438,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2435,10 +2446,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -2450,7 +2461,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2458,10 +2469,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2473,7 +2484,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2481,10 +2492,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D7" t="s">
         <v>142</v>
@@ -2496,7 +2507,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2504,13 +2515,13 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E8" t="s">
         <v>145</v>
@@ -2519,7 +2530,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update reports - 2026-01-30 11:55
</commit_message>
<xml_diff>
--- a/parliament_data.xlsx
+++ b/parliament_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="237">
   <si>
     <t>Publication ID</t>
   </si>
@@ -543,6 +543,30 @@
     <t>0:55:18</t>
   </si>
   <si>
+    <t>51336</t>
+  </si>
+  <si>
+    <t>HC 1658</t>
+  </si>
+  <si>
+    <t>Defence Committee</t>
+  </si>
+  <si>
+    <t>The UK contribution to European Security: Government Response</t>
+  </si>
+  <si>
+    <t>0:55:37</t>
+  </si>
+  <si>
+    <t>51345</t>
+  </si>
+  <si>
+    <t>HC 291-xlvi</t>
+  </si>
+  <si>
+    <t>Forty-sixth Report - 3 Statutory Instruments Reported</t>
+  </si>
+  <si>
     <t>Scan date</t>
   </si>
   <si>
@@ -625,6 +649,12 @@
   </si>
   <si>
     <t>10:59:37</t>
+  </si>
+  <si>
+    <t>11:55:37</t>
+  </si>
+  <si>
+    <t>51336, 51345</t>
   </si>
   <si>
     <t>Order Paper date</t>
@@ -744,8 +774,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reports" displayName="Reports" ref="A1:K33" totalsRowShown="0">
-  <autoFilter ref="A1:K33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reports" displayName="Reports" ref="A1:K35" totalsRowShown="0">
+  <autoFilter ref="A1:K35"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Publication ID"/>
     <tableColumn id="2" name="HC Number"/>
@@ -764,8 +794,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C20" totalsRowShown="0">
-  <autoFilter ref="A1:C20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scans" displayName="Scans" ref="A1:C21" totalsRowShown="0">
+  <autoFilter ref="A1:C21"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scan date"/>
     <tableColumn id="2" name="Scan time"/>
@@ -1077,7 +1107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2131,6 +2161,67 @@
       </c>
       <c r="K33" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>175</v>
+      </c>
+      <c r="B34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" t="s">
+        <v>177</v>
+      </c>
+      <c r="E34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" t="s">
+        <v>178</v>
+      </c>
+      <c r="G34" t="s">
+        <v>72</v>
+      </c>
+      <c r="H34" t="s">
+        <v>156</v>
+      </c>
+      <c r="I34" t="s">
+        <v>29</v>
+      </c>
+      <c r="K34" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
+        <v>180</v>
+      </c>
+      <c r="B35" t="s">
+        <v>181</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" t="s">
+        <v>182</v>
+      </c>
+      <c r="H35" t="s">
+        <v>156</v>
+      </c>
+      <c r="I35" t="s">
+        <v>29</v>
+      </c>
+      <c r="K35" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2143,7 +2234,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2151,13 +2242,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B1" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="C1" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2165,10 +2256,10 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2176,7 +2267,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2184,7 +2275,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2192,7 +2283,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2200,7 +2291,7 @@
         <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2208,7 +2299,7 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2216,10 +2307,10 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2227,7 +2318,7 @@
         <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2235,45 +2326,45 @@
         <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C10" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B11" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B12" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B13" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C13" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B14" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2281,10 +2372,10 @@
         <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="C15" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2292,7 +2383,7 @@
         <v>156</v>
       </c>
       <c r="B16" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2300,7 +2391,7 @@
         <v>156</v>
       </c>
       <c r="B17" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C17" t="s">
         <v>169</v>
@@ -2311,7 +2402,7 @@
         <v>156</v>
       </c>
       <c r="B18" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2319,7 +2410,7 @@
         <v>156</v>
       </c>
       <c r="B19" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2327,7 +2418,18 @@
         <v>156</v>
       </c>
       <c r="B20" t="s">
-        <v>202</v>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" t="s">
+        <v>211</v>
+      </c>
+      <c r="C21" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2348,28 +2450,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="F1" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="G1" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="H1" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2377,10 +2479,10 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="C2" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2392,7 +2494,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2400,10 +2502,10 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -2415,7 +2517,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2423,10 +2525,10 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
@@ -2438,7 +2540,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2446,10 +2548,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="C5" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -2461,7 +2563,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2469,10 +2571,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="C6" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2484,7 +2586,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2492,10 +2594,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="C7" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="D7" t="s">
         <v>142</v>
@@ -2507,7 +2609,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2515,13 +2617,13 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="C8" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="D8" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="E8" t="s">
         <v>145</v>
@@ -2530,7 +2632,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>